<commit_message>
Created PDF for the final project plan
</commit_message>
<xml_diff>
--- a/Diagrams/Project Plan.xlsx
+++ b/Diagrams/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\SBML-Converter-for-ERODE\Diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{68A11C29-F8D1-4E53-A542-EAEF8AAB9DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E8A125-1D2D-42F3-8233-4FAEF1FF0C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,6 +547,39 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -565,12 +598,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,33 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1019,7 +1019,7 @@
   <dimension ref="B1:BY21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1048,78 +1048,78 @@
       <c r="X1"/>
     </row>
     <row r="2" spans="2:77" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="10">
+        <v>18</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="27"/>
+      <c r="P2" s="36"/>
       <c r="Q2" s="13"/>
-      <c r="R2" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="29"/>
+      <c r="R2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="27"/>
       <c r="T2" s="14"/>
-      <c r="U2" s="28" t="s">
+      <c r="U2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
       <c r="Y2" s="15"/>
-      <c r="Z2" s="28" t="s">
+      <c r="Z2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="24"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="18"/>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17"/>
     </row>
     <row r="3" spans="2:77" s="7" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="30"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1184,12 +1184,12 @@
       <c r="BS3"/>
     </row>
     <row r="4" spans="2:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="19"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1246,452 +1246,452 @@
       </c>
       <c r="Z4"/>
       <c r="AA4"/>
-      <c r="BT4" s="31"/>
-      <c r="BU4" s="31"/>
-      <c r="BV4" s="31"/>
-      <c r="BW4" s="32"/>
-      <c r="BX4" s="32"/>
-      <c r="BY4" s="32"/>
+      <c r="BT4" s="20"/>
+      <c r="BU4" s="20"/>
+      <c r="BV4" s="20"/>
+      <c r="BW4" s="21"/>
+      <c r="BX4" s="21"/>
+      <c r="BY4" s="21"/>
     </row>
     <row r="5" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="34">
-        <v>1</v>
-      </c>
-      <c r="D5" s="34">
+      <c r="C5" s="23">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
         <v>4</v>
       </c>
-      <c r="E5" s="34">
-        <v>1</v>
-      </c>
-      <c r="F5" s="34">
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
         <v>4</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="24">
         <v>1</v>
       </c>
       <c r="Z5"/>
       <c r="AA5"/>
-      <c r="BT5" s="31"/>
-      <c r="BU5" s="31"/>
-      <c r="BV5" s="31"/>
-      <c r="BW5" s="32"/>
-      <c r="BX5" s="32"/>
-      <c r="BY5" s="32"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="21"/>
+      <c r="BX5" s="21"/>
+      <c r="BY5" s="21"/>
     </row>
     <row r="6" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="23">
         <v>2</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="23">
         <v>6</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="23">
         <v>2</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="23">
         <v>6</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="24">
         <v>1</v>
       </c>
       <c r="Z6"/>
       <c r="AA6"/>
-      <c r="BT6" s="31"/>
-      <c r="BU6" s="31"/>
-      <c r="BV6" s="31"/>
-      <c r="BW6" s="32"/>
-      <c r="BX6" s="32"/>
-      <c r="BY6" s="32"/>
+      <c r="BT6" s="20"/>
+      <c r="BU6" s="20"/>
+      <c r="BV6" s="20"/>
+      <c r="BW6" s="21"/>
+      <c r="BX6" s="21"/>
+      <c r="BY6" s="21"/>
     </row>
     <row r="7" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="23">
         <v>3</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="23">
         <v>2</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="23">
         <v>3</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="23">
         <v>4</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="24">
         <v>1</v>
       </c>
       <c r="Z7"/>
       <c r="AA7"/>
-      <c r="BT7" s="31"/>
-      <c r="BU7" s="31"/>
-      <c r="BV7" s="31"/>
-      <c r="BW7" s="32"/>
-      <c r="BX7" s="32"/>
-      <c r="BY7" s="32"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="20"/>
+      <c r="BW7" s="21"/>
+      <c r="BX7" s="21"/>
+      <c r="BY7" s="21"/>
     </row>
     <row r="8" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="23">
         <v>3</v>
       </c>
-      <c r="D8" s="34">
-        <v>1</v>
-      </c>
-      <c r="E8" s="34">
+      <c r="D8" s="23">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23">
         <v>3</v>
       </c>
-      <c r="F8" s="34">
-        <v>1</v>
-      </c>
-      <c r="G8" s="35">
+      <c r="F8" s="23">
+        <v>1</v>
+      </c>
+      <c r="G8" s="24">
         <v>1</v>
       </c>
       <c r="Z8"/>
       <c r="AA8"/>
-      <c r="BT8" s="31"/>
-      <c r="BU8" s="31"/>
-      <c r="BV8" s="31"/>
-      <c r="BW8" s="32"/>
-      <c r="BX8" s="32"/>
-      <c r="BY8" s="32"/>
+      <c r="BT8" s="20"/>
+      <c r="BU8" s="20"/>
+      <c r="BV8" s="20"/>
+      <c r="BW8" s="21"/>
+      <c r="BX8" s="21"/>
+      <c r="BY8" s="21"/>
     </row>
     <row r="9" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="23">
         <v>4</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="23">
         <v>2</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="23">
         <v>4</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="23">
         <v>7</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="24">
         <v>1</v>
       </c>
       <c r="Z9"/>
       <c r="AA9"/>
-      <c r="BT9" s="31"/>
-      <c r="BU9" s="31"/>
-      <c r="BV9" s="31"/>
-      <c r="BW9" s="32"/>
-      <c r="BX9" s="32"/>
-      <c r="BY9" s="32"/>
+      <c r="BT9" s="20"/>
+      <c r="BU9" s="20"/>
+      <c r="BV9" s="20"/>
+      <c r="BW9" s="21"/>
+      <c r="BX9" s="21"/>
+      <c r="BY9" s="21"/>
     </row>
     <row r="10" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="23">
         <v>6</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="23">
         <v>2</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="23">
         <v>6</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="23">
         <v>6</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="24">
         <v>1</v>
       </c>
       <c r="Z10"/>
       <c r="AA10"/>
-      <c r="BT10" s="31"/>
-      <c r="BU10" s="31"/>
-      <c r="BV10" s="31"/>
-      <c r="BW10" s="32"/>
-      <c r="BX10" s="32"/>
-      <c r="BY10" s="32"/>
+      <c r="BT10" s="20"/>
+      <c r="BU10" s="20"/>
+      <c r="BV10" s="20"/>
+      <c r="BW10" s="21"/>
+      <c r="BX10" s="21"/>
+      <c r="BY10" s="21"/>
     </row>
     <row r="11" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="23">
         <v>6</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="23">
         <v>2</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="23">
         <v>6</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="23">
         <v>6</v>
       </c>
-      <c r="G11" s="35">
+      <c r="G11" s="24">
         <v>1</v>
       </c>
       <c r="Z11"/>
       <c r="AA11"/>
-      <c r="BT11" s="31"/>
-      <c r="BU11" s="31"/>
-      <c r="BV11" s="31"/>
-      <c r="BW11" s="32"/>
-      <c r="BX11" s="32"/>
-      <c r="BY11" s="32"/>
+      <c r="BT11" s="20"/>
+      <c r="BU11" s="20"/>
+      <c r="BV11" s="20"/>
+      <c r="BW11" s="21"/>
+      <c r="BX11" s="21"/>
+      <c r="BY11" s="21"/>
     </row>
     <row r="12" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="23">
         <v>9</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="23">
         <v>2</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="23">
         <v>11</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="23">
         <v>2</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G12" s="24">
         <v>1</v>
       </c>
       <c r="Z12"/>
       <c r="AA12"/>
-      <c r="BT12" s="31"/>
-      <c r="BU12" s="31"/>
-      <c r="BV12" s="31"/>
-      <c r="BW12" s="32"/>
-      <c r="BX12" s="32"/>
-      <c r="BY12" s="32"/>
+      <c r="BT12" s="20"/>
+      <c r="BU12" s="20"/>
+      <c r="BV12" s="20"/>
+      <c r="BW12" s="21"/>
+      <c r="BX12" s="21"/>
+      <c r="BY12" s="21"/>
     </row>
     <row r="13" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13" s="23">
         <v>10</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="23">
         <v>2</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="23">
         <v>11</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="23">
         <v>2</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="24">
         <v>1</v>
       </c>
       <c r="Z13"/>
       <c r="AA13"/>
-      <c r="BT13" s="31"/>
-      <c r="BU13" s="31"/>
-      <c r="BV13" s="31"/>
-      <c r="BW13" s="32"/>
-      <c r="BX13" s="32"/>
-      <c r="BY13" s="32"/>
+      <c r="BT13" s="20"/>
+      <c r="BU13" s="20"/>
+      <c r="BV13" s="20"/>
+      <c r="BW13" s="21"/>
+      <c r="BX13" s="21"/>
+      <c r="BY13" s="21"/>
     </row>
     <row r="14" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="25">
         <v>13</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="23">
         <v>3</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="23">
         <v>13</v>
       </c>
-      <c r="F14" s="34">
+      <c r="F14" s="23">
         <v>3</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="24">
         <v>1</v>
       </c>
       <c r="Z14"/>
       <c r="AA14"/>
-      <c r="BT14" s="31"/>
-      <c r="BU14" s="31"/>
-      <c r="BV14" s="31"/>
-      <c r="BW14" s="32"/>
-      <c r="BX14" s="32"/>
-      <c r="BY14" s="32"/>
+      <c r="BT14" s="20"/>
+      <c r="BU14" s="20"/>
+      <c r="BV14" s="20"/>
+      <c r="BW14" s="21"/>
+      <c r="BX14" s="21"/>
+      <c r="BY14" s="21"/>
     </row>
     <row r="15" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="23">
         <v>13</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="23">
         <v>3</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="23">
         <v>13</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="23">
         <v>3</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="24">
         <v>1</v>
       </c>
       <c r="Z15"/>
       <c r="AA15"/>
-      <c r="BT15" s="31"/>
-      <c r="BU15" s="31"/>
-      <c r="BV15" s="31"/>
-      <c r="BW15" s="32"/>
-      <c r="BX15" s="32"/>
-      <c r="BY15" s="32"/>
+      <c r="BT15" s="20"/>
+      <c r="BU15" s="20"/>
+      <c r="BV15" s="20"/>
+      <c r="BW15" s="21"/>
+      <c r="BX15" s="21"/>
+      <c r="BY15" s="21"/>
     </row>
     <row r="16" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="23">
         <v>13</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="23">
         <v>4</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="23">
         <v>13</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F16" s="23">
         <v>4</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="24">
         <v>1</v>
       </c>
       <c r="Z16"/>
       <c r="AA16"/>
-      <c r="BT16" s="31"/>
-      <c r="BU16" s="31"/>
-      <c r="BV16" s="31"/>
-      <c r="BW16" s="32"/>
-      <c r="BX16" s="32"/>
-      <c r="BY16" s="32"/>
+      <c r="BT16" s="20"/>
+      <c r="BU16" s="20"/>
+      <c r="BV16" s="20"/>
+      <c r="BW16" s="21"/>
+      <c r="BX16" s="21"/>
+      <c r="BY16" s="21"/>
     </row>
     <row r="17" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="23">
         <v>14</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="23">
         <v>3</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="23">
         <v>14</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="23">
         <v>3</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="24">
         <v>1</v>
       </c>
       <c r="Z17"/>
       <c r="AA17"/>
-      <c r="BT17" s="31"/>
-      <c r="BU17" s="31"/>
-      <c r="BV17" s="31"/>
-      <c r="BW17" s="32"/>
-      <c r="BX17" s="32"/>
-      <c r="BY17" s="32"/>
+      <c r="BT17" s="20"/>
+      <c r="BU17" s="20"/>
+      <c r="BV17" s="20"/>
+      <c r="BW17" s="21"/>
+      <c r="BX17" s="21"/>
+      <c r="BY17" s="21"/>
     </row>
     <row r="18" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="23">
         <v>15</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="23">
         <v>2</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="23">
         <v>15</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="23">
         <v>2</v>
       </c>
-      <c r="G18" s="35">
-        <v>0.5</v>
+      <c r="G18" s="24">
+        <v>1</v>
       </c>
       <c r="Z18"/>
       <c r="AA18"/>
-      <c r="BT18" s="31"/>
-      <c r="BU18" s="31"/>
-      <c r="BV18" s="31"/>
-      <c r="BW18" s="32"/>
-      <c r="BX18" s="32"/>
-      <c r="BY18" s="32"/>
+      <c r="BT18" s="20"/>
+      <c r="BU18" s="20"/>
+      <c r="BV18" s="20"/>
+      <c r="BW18" s="21"/>
+      <c r="BX18" s="21"/>
+      <c r="BY18" s="21"/>
     </row>
     <row r="19" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="34">
+      <c r="C19" s="23">
         <v>16</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="23">
         <v>3</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="23">
         <v>16</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="23">
         <v>3</v>
       </c>
-      <c r="G19" s="35">
-        <v>0.5</v>
+      <c r="G19" s="24">
+        <v>1</v>
       </c>
       <c r="Z19"/>
       <c r="AA19"/>
-      <c r="BT19" s="31"/>
-      <c r="BU19" s="31"/>
-      <c r="BV19" s="31"/>
-      <c r="BW19" s="32"/>
-      <c r="BX19" s="32"/>
-      <c r="BY19" s="32"/>
+      <c r="BT19" s="20"/>
+      <c r="BU19" s="20"/>
+      <c r="BV19" s="20"/>
+      <c r="BW19" s="21"/>
+      <c r="BX19" s="21"/>
+      <c r="BY19" s="21"/>
     </row>
     <row r="20" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Z20"/>
       <c r="AA20"/>
-      <c r="BT20" s="31"/>
-      <c r="BU20" s="31"/>
-      <c r="BV20" s="31"/>
-      <c r="BW20" s="32"/>
-      <c r="BX20" s="32"/>
-      <c r="BY20" s="32"/>
+      <c r="BT20" s="20"/>
+      <c r="BU20" s="20"/>
+      <c r="BV20" s="20"/>
+      <c r="BW20" s="21"/>
+      <c r="BX20" s="21"/>
+      <c r="BY20" s="21"/>
     </row>
     <row r="21" spans="2:77" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="Z21"/>
       <c r="AA21"/>
-      <c r="BT21" s="31"/>
-      <c r="BU21" s="31"/>
-      <c r="BV21" s="31"/>
-      <c r="BW21" s="32"/>
-      <c r="BX21" s="32"/>
-      <c r="BY21" s="32"/>
+      <c r="BT21" s="20"/>
+      <c r="BU21" s="20"/>
+      <c r="BV21" s="20"/>
+      <c r="BW21" s="21"/>
+      <c r="BX21" s="21"/>
+      <c r="BY21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>